<commit_message>
updated BGPmon set with new data
</commit_message>
<xml_diff>
--- a/data/Malicious Routing Shortlist.xlsx
+++ b/data/Malicious Routing Shortlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikna\Desktop\Politics of Routing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE735296-779E-4012-BC28-661C75099543}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0EB290-0EBB-4A01-B5B8-F53F17E53DDC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="445">
   <si>
     <t>AD</t>
   </si>
@@ -1916,10 +1916,10 @@
       <totalsRowFormula>SUM(B2:B66)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{CB08F8B3-73D8-4C99-A366-FA8017EE0D03}" name="Mirai-Like Normalised"/>
-    <tableColumn id="3" xr3:uid="{EDB869B8-F2B6-4CDA-8A98-BD6AC8DFF553}" name="BGP Hijacks" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(D2:D66)</totalsRowFormula>
+    <tableColumn id="9" xr3:uid="{073C29FB-BAA7-451E-AA1E-76930F6E46F7}" name="BGP Hijacks"/>
+    <tableColumn id="10" xr3:uid="{036D57D5-B326-42ED-8FFD-747DA6B50910}" name="BGP Hijacks Normalised">
+      <calculatedColumnFormula>D2/384</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0B1B2928-734D-4499-AE64-9A49F650C8A5}" name="BGP Hijacks Normalised"/>
     <tableColumn id="4" xr3:uid="{3A0FA3E4-0714-48E9-A35A-76BB86EBC367}" name="Using Chinese Training"/>
     <tableColumn id="5" xr3:uid="{E8D3BBBC-FD07-4637-8DED-2FE5C7491C7E}" name="Citizens arrested over political social media posts"/>
     <tableColumn id="6" xr3:uid="{0A948547-E070-4D9E-A4DC-3394201B9DF2}" name="Any Internet/Telecom mass surveillance"/>
@@ -1931,14 +1931,14 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3F186C1-4BC8-4073-9AAE-9C4BD46845C3}" name="Table1" displayName="Table1" ref="A1:D1048576" totalsRowShown="0">
   <autoFilter ref="A1:D1048576" xr:uid="{07CFB2B1-7468-43FC-A356-3280593350B7}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D213">
-    <sortCondition ref="B1:B1048576"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C214">
+    <sortCondition ref="A1:A1048576"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1C986861-56D1-4778-9305-7A4F9495C70B}" name="Code"/>
     <tableColumn id="2" xr3:uid="{21B3926C-46C0-4B40-9817-7EF772684984}" name="Country"/>
     <tableColumn id="3" xr3:uid="{314CC48B-B6D0-415C-B007-5793AF1A3CCD}" name="Mirai-like Hits"/>
-    <tableColumn id="4" xr3:uid="{C2D494FE-6D34-4AA5-82F6-47F4380202CE}" name="BGP Hijacks"/>
+    <tableColumn id="5" xr3:uid="{DA70B094-2CEF-4139-BAAA-79E202110E60}" name="BGP Hijacks"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2244,15 +2244,13 @@
   <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="2" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="25.28515625" customWidth="1"/>
     <col min="8" max="8" width="26.7109375" customWidth="1"/>
@@ -2295,10 +2293,11 @@
         <v>1.7699115044247788E-4</v>
       </c>
       <c r="D2">
-        <v>308</v>
+        <v>77</v>
       </c>
       <c r="E2">
-        <v>0.48580441640378547</v>
+        <f>D2/384</f>
+        <v>0.20052083333333334</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -2321,10 +2320,11 @@
         <v>4.2418879056047194E-2</v>
       </c>
       <c r="D3">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E3">
-        <v>2.0504731861198739E-2</v>
+        <f t="shared" ref="E3:E66" si="0">D3/384</f>
+        <v>4.4270833333333336E-2</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2350,6 +2350,7 @@
         <v>0</v>
       </c>
       <c r="E4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4">
@@ -2373,10 +2374,11 @@
         <v>1.1032448377581121E-2</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.8229166666666668E-2</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -2402,6 +2404,7 @@
         <v>0</v>
       </c>
       <c r="E6">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F6">
@@ -2425,10 +2428,11 @@
         <v>8.0629301868239919E-4</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.6041666666666665E-3</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2451,10 +2455,11 @@
         <v>4.7787610619469028E-3</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.2916666666666671E-2</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -2477,10 +2482,11 @@
         <v>1.2389380530973451E-3</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>1.2618296529968454E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -2503,10 +2509,11 @@
         <v>0.1775417895771878</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.27864583333333331</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -2529,10 +2536,11 @@
         <v>1.3569321533923305E-3</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.3020833333333334E-2</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -2555,10 +2563,11 @@
         <v>2.2241887905604718E-2</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.6875E-2</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -2581,10 +2590,11 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.21875</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -2607,10 +2617,11 @@
         <v>1.4886922320550638E-2</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.3020833333333334E-2</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -2636,6 +2647,7 @@
         <v>0</v>
       </c>
       <c r="E15">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15">
@@ -2659,10 +2671,11 @@
         <v>1.2035398230088496E-2</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.5625E-2</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -2685,10 +2698,11 @@
         <v>0.21789577187807277</v>
       </c>
       <c r="D17">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>1.8927444794952682E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.5625E-2</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -2711,10 +2725,11 @@
         <v>4.5231071779744348E-4</v>
       </c>
       <c r="D18">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E18">
-        <v>1.4195583596214511E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.8229166666666668E-2</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -2737,10 +2752,11 @@
         <v>1.5142576204523108E-3</v>
       </c>
       <c r="D19">
-        <v>420</v>
+        <v>107</v>
       </c>
       <c r="E19">
-        <v>0.66246056782334384</v>
+        <f t="shared" si="0"/>
+        <v>0.27864583333333331</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -2763,10 +2779,11 @@
         <v>2.4287118977384465E-2</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6.7708333333333329E-2</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -2792,6 +2809,7 @@
         <v>0</v>
       </c>
       <c r="E21">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F21">
@@ -2815,10 +2833,11 @@
         <v>2.9891838741396264E-3</v>
       </c>
       <c r="D22">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="E22">
-        <v>5.5205047318611984E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.8645833333333332E-2</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -2841,10 +2860,11 @@
         <v>2.6607669616519173E-2</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.16927083333333334</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -2867,10 +2887,11 @@
         <v>1.1976401179941002E-2</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.8125E-3</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -2893,10 +2914,11 @@
         <v>1.9665683382497542E-4</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.6041666666666665E-3</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -2919,10 +2941,11 @@
         <v>6.3284169124877096E-2</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.25</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -2945,10 +2968,11 @@
         <v>5.9449360865290068E-2</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -2974,6 +2998,7 @@
         <v>0</v>
       </c>
       <c r="E28">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F28">
@@ -2997,10 +3022,11 @@
         <v>5.663716814159292E-2</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.34375E-2</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -3023,10 +3049,11 @@
         <v>0.19301868239921338</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -3049,10 +3076,11 @@
         <v>2.910521140609636E-3</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>3.1545741324921135E-3</v>
+        <f t="shared" si="0"/>
+        <v>2.6041666666666665E-3</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -3075,10 +3103,11 @@
         <v>4.7394296951819076E-3</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.208333333333333E-3</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -3101,10 +3130,11 @@
         <v>5.1130776794493606E-4</v>
       </c>
       <c r="D33">
-        <v>131</v>
+        <v>34</v>
       </c>
       <c r="E33">
-        <v>0.20662460567823343</v>
+        <f t="shared" si="0"/>
+        <v>8.8541666666666671E-2</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -3127,10 +3157,11 @@
         <v>2.5565388397246803E-4</v>
       </c>
       <c r="D34">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E34">
-        <v>4.8895899053627762E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.8645833333333332E-2</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -3153,10 +3184,11 @@
         <v>2.3598820058997051E-4</v>
       </c>
       <c r="D35">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E35">
-        <v>8.9905362776025233E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.7291666666666664E-2</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -3182,6 +3214,7 @@
         <v>0</v>
       </c>
       <c r="E36">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F36">
@@ -3205,10 +3238,11 @@
         <v>1.9665683382497542E-5</v>
       </c>
       <c r="D37">
-        <v>165</v>
+        <v>41</v>
       </c>
       <c r="E37">
-        <v>0.26025236593059936</v>
+        <f t="shared" si="0"/>
+        <v>0.10677083333333333</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -3231,10 +3265,11 @@
         <v>2.4857423795476893E-2</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.34375E-2</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -3257,10 +3292,11 @@
         <v>9.176007866273353E-2</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -3283,10 +3319,11 @@
         <v>3.2723697148475908E-2</v>
       </c>
       <c r="D40">
-        <v>634</v>
+        <v>160</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.41666666666666669</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -3312,6 +3349,7 @@
         <v>0</v>
       </c>
       <c r="E41">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F41">
@@ -3335,10 +3373,11 @@
         <v>1.6007866273352999E-2</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.6041666666666665E-3</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -3361,10 +3400,11 @@
         <v>1.2015732546705998E-2</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.8229166666666668E-2</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -3387,10 +3427,11 @@
         <v>5.0344149459193707E-3</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.8229166666666668E-2</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -3416,6 +3457,7 @@
         <v>0</v>
       </c>
       <c r="E45">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F45">
@@ -3442,6 +3484,7 @@
         <v>0</v>
       </c>
       <c r="E46">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F46">
@@ -3465,10 +3508,11 @@
         <v>4.0707964601769909E-3</v>
       </c>
       <c r="D47">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E47">
-        <v>8.3596214511041003E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.4270833333333336E-2</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -3491,10 +3535,11 @@
         <v>2.6705998033431662E-2</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.6458333333333336E-2</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -3517,10 +3562,11 @@
         <v>1.3215339233038349E-2</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E49">
-        <v>4.7318611987381704E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.4270833333333336E-2</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -3546,6 +3592,7 @@
         <v>0</v>
       </c>
       <c r="E50">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F50">
@@ -3569,10 +3616,11 @@
         <v>1.415929203539823E-3</v>
       </c>
       <c r="D51">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E51">
-        <v>6.1514195583596214E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.8645833333333332E-2</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -3595,10 +3643,11 @@
         <v>1.5732546705998033E-4</v>
       </c>
       <c r="D52">
-        <v>161</v>
+        <v>40</v>
       </c>
       <c r="E52">
-        <v>0.25394321766561512</v>
+        <f t="shared" si="0"/>
+        <v>0.10416666666666667</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -3624,6 +3673,7 @@
         <v>0</v>
       </c>
       <c r="E53">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F53">
@@ -3647,10 +3697,11 @@
         <v>3.478859390363815E-2</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.8125E-3</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -3673,10 +3724,11 @@
         <v>8.2595870206489674E-3</v>
       </c>
       <c r="D55">
-        <v>451</v>
+        <v>113</v>
       </c>
       <c r="E55">
-        <v>0.71135646687697163</v>
+        <f t="shared" si="0"/>
+        <v>0.29427083333333331</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -3699,10 +3751,11 @@
         <v>0.10007866273352999</v>
       </c>
       <c r="D56">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E56">
-        <v>3.3123028391167195E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.3854166666666664E-2</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -3725,10 +3778,11 @@
         <v>1.7699115044247788E-4</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E57">
-        <v>3.1545741324921135E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.3020833333333334E-2</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -3751,10 +3805,11 @@
         <v>2.6135693215339234E-2</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6.7708333333333329E-2</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -3777,10 +3832,11 @@
         <v>8.4169124877089482E-3</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.208333333333333E-3</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -3803,10 +3859,11 @@
         <v>2.9124877089478859E-2</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.25520833333333331</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -3829,10 +3886,11 @@
         <v>0.19065880039331368</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>384</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -3855,10 +3913,11 @@
         <v>3.9331366764995085E-4</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.6041666666666665E-3</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -3881,10 +3940,11 @@
         <v>1.7266470009832842E-2</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.6041666666666665E-3</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -3910,6 +3970,7 @@
         <v>0</v>
       </c>
       <c r="E64">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F64">
@@ -3933,10 +3994,11 @@
         <v>4.1297935103244839E-4</v>
       </c>
       <c r="D65">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E65">
-        <v>3.3123028391167195E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.3020833333333334E-2</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -3959,10 +4021,11 @@
         <v>0</v>
       </c>
       <c r="D66">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="E66">
-        <v>0.13722397476340695</v>
+        <f t="shared" si="0"/>
+        <v>5.7291666666666664E-2</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -3978,10 +4041,6 @@
       <c r="B67">
         <f>SUM(B2:B66)</f>
         <v>132342</v>
-      </c>
-      <c r="D67">
-        <f>SUM(D2:D66)</f>
-        <v>2663</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -4008,8 +4067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2413B972-2BB9-41F4-8DD9-22C30F350830}">
   <dimension ref="A1:D213"/>
   <sheetViews>
-    <sheetView topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4017,7 +4076,7 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.140625" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -4036,100 +4095,100 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>75</v>
+        <v>428</v>
       </c>
       <c r="D3">
-        <v>147</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>372</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>402</v>
-      </c>
-      <c r="C5" t="s">
-        <v>401</v>
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>13</v>
       </c>
       <c r="D5">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>401</v>
+        <v>75</v>
+      </c>
+      <c r="D6">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="D7">
-        <v>308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>401</v>
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4143,35 +4202,35 @@
         <v>2157</v>
       </c>
       <c r="D9">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>372</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>168</v>
-      </c>
-      <c r="D10" t="s">
+        <v>402</v>
+      </c>
+      <c r="C10" t="s">
         <v>401</v>
+      </c>
+      <c r="D10">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>401</v>
+        <v>237</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4184,22 +4243,22 @@
       <c r="C12">
         <v>561</v>
       </c>
-      <c r="D12" t="s">
-        <v>401</v>
+      <c r="D12">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C13">
-        <v>237</v>
-      </c>
-      <c r="D13" t="s">
-        <v>401</v>
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -4212,36 +4271,36 @@
       <c r="C14">
         <v>44</v>
       </c>
-      <c r="D14" t="s">
-        <v>401</v>
+      <c r="D14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C15">
-        <v>33</v>
+        <v>118</v>
       </c>
       <c r="D15">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C16">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>401</v>
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4254,148 +4313,148 @@
       <c r="C17">
         <v>243</v>
       </c>
-      <c r="D17" t="s">
-        <v>401</v>
+      <c r="D17">
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C18">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s">
-        <v>401</v>
+        <v>211</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C19">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C20">
-        <v>211</v>
-      </c>
-      <c r="D20" t="s">
-        <v>401</v>
+        <v>1786</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="C21">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>401</v>
+        <v>41</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D22">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>401</v>
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C24">
-        <v>138</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>401</v>
+        <v>14</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C26">
-        <v>118</v>
-      </c>
-      <c r="D26" t="s">
-        <v>401</v>
+        <v>138</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C27">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4408,932 +4467,932 @@
       <c r="C28">
         <v>9028</v>
       </c>
-      <c r="D28" t="s">
-        <v>401</v>
+      <c r="D28">
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>377</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>407</v>
-      </c>
-      <c r="C29" t="s">
-        <v>401</v>
+        <v>53</v>
+      </c>
+      <c r="C29">
+        <v>33</v>
       </c>
       <c r="D29">
-        <v>62</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>360</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>361</v>
+        <v>55</v>
       </c>
       <c r="C30">
-        <v>3</v>
-      </c>
-      <c r="D30" t="s">
-        <v>401</v>
+        <v>16</v>
+      </c>
+      <c r="D30">
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C31">
-        <v>14</v>
-      </c>
-      <c r="D31" t="s">
-        <v>401</v>
+        <v>63</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C32">
-        <v>1786</v>
+        <v>6</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>1131</v>
       </c>
       <c r="D33">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>373</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34" t="s">
+        <v>403</v>
+      </c>
+      <c r="C34" t="s">
         <v>401</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>177</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>178</v>
+        <v>63</v>
       </c>
       <c r="C35">
-        <v>69</v>
-      </c>
-      <c r="D35" t="s">
-        <v>401</v>
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C36">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="D36">
-        <v>111</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C37">
-        <v>1131</v>
-      </c>
-      <c r="D37" t="s">
-        <v>401</v>
+        <v>18</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>374</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>404</v>
-      </c>
-      <c r="C38" t="s">
-        <v>401</v>
+        <v>69</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
       </c>
       <c r="D38">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>183</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>184</v>
+        <v>71</v>
       </c>
       <c r="C39">
-        <v>5</v>
-      </c>
-      <c r="D39" t="s">
-        <v>401</v>
+        <v>802</v>
+      </c>
+      <c r="D39">
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>373</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>403</v>
-      </c>
-      <c r="C40" t="s">
-        <v>401</v>
+        <v>73</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
       </c>
       <c r="D40">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>419</v>
-      </c>
-      <c r="C41" t="s">
-        <v>401</v>
+        <v>75</v>
+      </c>
+      <c r="C41">
+        <v>50850</v>
       </c>
       <c r="D41">
-        <v>68</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C42">
-        <v>802</v>
-      </c>
-      <c r="D42" t="s">
-        <v>401</v>
+        <v>757</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C43">
-        <v>50850</v>
-      </c>
-      <c r="D43" t="s">
-        <v>401</v>
+        <v>141</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>374</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
-      </c>
-      <c r="C44">
-        <v>757</v>
-      </c>
-      <c r="D44" t="s">
+        <v>404</v>
+      </c>
+      <c r="C44" t="s">
         <v>401</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>380</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>410</v>
-      </c>
-      <c r="C45" t="s">
-        <v>401</v>
+        <v>81</v>
+      </c>
+      <c r="C45">
+        <v>12</v>
       </c>
       <c r="D45">
-        <v>179</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>157</v>
       </c>
       <c r="D46">
-        <v>357</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>527</v>
       </c>
       <c r="D47">
-        <v>51</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C48">
-        <v>141</v>
-      </c>
-      <c r="D48" t="s">
-        <v>401</v>
+        <v>1353</v>
+      </c>
+      <c r="D48">
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="C49">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>145</v>
+        <v>90</v>
       </c>
       <c r="B50" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
       <c r="C50">
-        <v>124</v>
-      </c>
-      <c r="D50" t="s">
-        <v>401</v>
+        <v>260</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C51">
-        <v>12</v>
-      </c>
-      <c r="D51" t="s">
-        <v>401</v>
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C52">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="D52">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C53">
-        <v>527</v>
-      </c>
-      <c r="D53" t="s">
-        <v>401</v>
+        <v>13</v>
+      </c>
+      <c r="D53">
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B54" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C54">
-        <v>260</v>
-      </c>
-      <c r="D54" t="s">
-        <v>401</v>
+        <v>612</v>
+      </c>
+      <c r="D54">
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C55">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D55">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B56" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56" t="s">
-        <v>401</v>
+        <v>11080</v>
+      </c>
+      <c r="D56">
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B57" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C57">
-        <v>183</v>
+        <v>1454</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C58">
-        <v>612</v>
-      </c>
-      <c r="D58" t="s">
-        <v>401</v>
+        <v>77</v>
+      </c>
+      <c r="D58">
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B59" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C59">
-        <v>11080</v>
+        <v>113</v>
       </c>
       <c r="D59">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>321</v>
+        <v>110</v>
       </c>
       <c r="B60" t="s">
-        <v>322</v>
+        <v>111</v>
       </c>
       <c r="C60">
         <v>15</v>
       </c>
       <c r="D60">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>375</v>
       </c>
       <c r="B61" t="s">
-        <v>132</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
+        <v>405</v>
+      </c>
+      <c r="C61" t="s">
+        <v>401</v>
       </c>
       <c r="D61">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C62">
-        <v>23</v>
+        <v>1235</v>
       </c>
       <c r="D62">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C63">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="D63">
-        <v>420</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>375</v>
+        <v>116</v>
       </c>
       <c r="B64" t="s">
-        <v>405</v>
-      </c>
-      <c r="C64" t="s">
-        <v>401</v>
+        <v>436</v>
+      </c>
+      <c r="C64">
+        <v>1481</v>
       </c>
       <c r="D64">
-        <v>19</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B65" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C65">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D65">
-        <v>104</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B66" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C66">
-        <v>113</v>
-      </c>
-      <c r="D66" t="s">
-        <v>401</v>
+        <v>152</v>
+      </c>
+      <c r="D66">
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B67" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="C67">
-        <v>1235</v>
-      </c>
-      <c r="D67" t="s">
-        <v>401</v>
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B68" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C68">
-        <v>1</v>
-      </c>
-      <c r="D68" t="s">
-        <v>401</v>
+        <v>15</v>
+      </c>
+      <c r="D68">
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>267</v>
+        <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>268</v>
+        <v>126</v>
       </c>
       <c r="C69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="B70" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C70">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D70">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B71" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C71">
-        <v>6</v>
-      </c>
-      <c r="D71" t="s">
-        <v>401</v>
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B72" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C72">
-        <v>152</v>
+        <v>1</v>
       </c>
       <c r="D72">
-        <v>35</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="B73" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="C73">
-        <v>1353</v>
-      </c>
-      <c r="D73" t="s">
-        <v>401</v>
+        <v>1604</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>123</v>
+        <v>376</v>
       </c>
       <c r="B74" t="s">
-        <v>124</v>
-      </c>
-      <c r="C74">
-        <v>15</v>
+        <v>406</v>
+      </c>
+      <c r="C74" t="s">
+        <v>401</v>
       </c>
       <c r="D74">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B75" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C75">
+        <v>24</v>
+      </c>
+      <c r="D75">
         <v>3</v>
-      </c>
-      <c r="D75" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B76" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C76">
-        <v>1604</v>
-      </c>
-      <c r="D76" t="s">
-        <v>401</v>
+        <v>15</v>
+      </c>
+      <c r="D76">
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="B77" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="C77">
+        <v>69</v>
+      </c>
+      <c r="D77">
         <v>3</v>
-      </c>
-      <c r="D77">
-        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B78" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C78">
-        <v>15</v>
+        <v>4021</v>
       </c>
       <c r="D78">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B79" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C79">
-        <v>24</v>
-      </c>
-      <c r="D79" t="s">
-        <v>401</v>
+        <v>42</v>
+      </c>
+      <c r="D79">
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="B80" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="C80">
-        <v>1</v>
-      </c>
-      <c r="D80" t="s">
-        <v>401</v>
+        <v>124</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B81" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="C81">
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="D81">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B82" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C82">
-        <v>6</v>
+        <v>609</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B83" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C83">
-        <v>42</v>
-      </c>
-      <c r="D83" t="s">
-        <v>401</v>
+        <v>3023</v>
+      </c>
+      <c r="D83">
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="B84" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="C84">
-        <v>4021</v>
-      </c>
-      <c r="D84" t="s">
-        <v>401</v>
+        <v>118</v>
+      </c>
+      <c r="D84">
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B85" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C85">
-        <v>609</v>
-      </c>
-      <c r="D85" t="s">
-        <v>401</v>
+        <v>470</v>
+      </c>
+      <c r="D85">
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B86" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C86">
-        <v>10</v>
-      </c>
-      <c r="D86" t="s">
-        <v>401</v>
+        <v>3218</v>
+      </c>
+      <c r="D86">
+        <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>157</v>
+        <v>377</v>
       </c>
       <c r="B87" t="s">
-        <v>158</v>
-      </c>
-      <c r="C87">
-        <v>3218</v>
-      </c>
-      <c r="D87" t="s">
+        <v>407</v>
+      </c>
+      <c r="C87" t="s">
         <v>401</v>
+      </c>
+      <c r="D87">
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B88" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="C88">
-        <v>3023</v>
-      </c>
-      <c r="D88" t="s">
-        <v>401</v>
+        <v>45</v>
+      </c>
+      <c r="D88">
+        <v>176</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B89" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C89">
-        <v>45</v>
+        <v>729</v>
       </c>
       <c r="D89">
-        <v>665</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="B90" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C90">
-        <v>118</v>
-      </c>
-      <c r="D90" t="s">
-        <v>401</v>
+        <v>10</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B91" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C91">
-        <v>729</v>
+        <v>2880</v>
       </c>
       <c r="D91">
-        <v>117</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>155</v>
+        <v>378</v>
       </c>
       <c r="B92" t="s">
-        <v>156</v>
-      </c>
-      <c r="C92">
-        <v>470</v>
+        <v>408</v>
+      </c>
+      <c r="C92" t="s">
+        <v>401</v>
       </c>
       <c r="D92">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B93" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C93">
-        <v>2880</v>
-      </c>
-      <c r="D93" t="s">
-        <v>401</v>
+        <v>28</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B94" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C94">
-        <v>28</v>
-      </c>
-      <c r="D94" t="s">
-        <v>401</v>
+        <v>148</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -5346,78 +5405,78 @@
       <c r="C95">
         <v>9815</v>
       </c>
-      <c r="D95" t="s">
-        <v>401</v>
+      <c r="D95">
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>378</v>
+        <v>173</v>
       </c>
       <c r="B96" t="s">
-        <v>408</v>
-      </c>
-      <c r="C96" t="s">
-        <v>401</v>
+        <v>174</v>
+      </c>
+      <c r="C96">
+        <v>26</v>
       </c>
       <c r="D96">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C97">
-        <v>148</v>
+        <v>13</v>
       </c>
       <c r="D97">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B98" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C98">
-        <v>241</v>
-      </c>
-      <c r="D98" t="s">
-        <v>401</v>
+        <v>69</v>
+      </c>
+      <c r="D98">
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>173</v>
+        <v>379</v>
       </c>
       <c r="B99" t="s">
-        <v>174</v>
-      </c>
-      <c r="C99">
-        <v>26</v>
+        <v>409</v>
+      </c>
+      <c r="C99" t="s">
+        <v>401</v>
       </c>
       <c r="D99">
-        <v>131</v>
+        <v>107</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B100" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C100" t="s">
         <v>401</v>
       </c>
       <c r="D100">
-        <v>427</v>
+        <v>45</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -5431,7 +5490,7 @@
         <v>401</v>
       </c>
       <c r="D101">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -5444,8 +5503,8 @@
       <c r="C102">
         <v>6397</v>
       </c>
-      <c r="D102" t="s">
-        <v>401</v>
+      <c r="D102">
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -5459,49 +5518,49 @@
         <v>199</v>
       </c>
       <c r="D103">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B104" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C104">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D104">
-        <v>31</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B105" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C105">
-        <v>10</v>
-      </c>
-      <c r="D105" t="s">
-        <v>401</v>
+        <v>241</v>
+      </c>
+      <c r="D105">
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B106" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="C106">
-        <v>168</v>
-      </c>
-      <c r="D106" t="s">
-        <v>401</v>
+        <v>10</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -5515,18 +5574,18 @@
         <v>12</v>
       </c>
       <c r="D107">
-        <v>57</v>
+        <v>22</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>382</v>
+        <v>191</v>
       </c>
       <c r="B108" t="s">
-        <v>412</v>
-      </c>
-      <c r="C108" t="s">
-        <v>401</v>
+        <v>192</v>
+      </c>
+      <c r="C108">
+        <v>6</v>
       </c>
       <c r="D108">
         <v>3</v>
@@ -5534,422 +5593,422 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B109" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C109">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="D109">
-        <v>67</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B110" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C110">
-        <v>2</v>
-      </c>
-      <c r="D110" t="s">
-        <v>401</v>
+        <v>1</v>
+      </c>
+      <c r="D110">
+        <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>197</v>
+        <v>382</v>
       </c>
       <c r="B111" t="s">
-        <v>198</v>
-      </c>
-      <c r="C111">
-        <v>84</v>
+        <v>412</v>
+      </c>
+      <c r="C111" t="s">
+        <v>401</v>
       </c>
       <c r="D111">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B112" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C112">
-        <v>17</v>
-      </c>
-      <c r="D112" t="s">
-        <v>401</v>
+        <v>84</v>
+      </c>
+      <c r="D112">
+        <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
       <c r="B113" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="C113">
-        <v>97</v>
-      </c>
-      <c r="D113" t="s">
-        <v>401</v>
+        <v>17</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="B114" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="C114">
-        <v>84</v>
-      </c>
-      <c r="D114" t="s">
-        <v>401</v>
+        <v>168</v>
+      </c>
+      <c r="D114">
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B115" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C115">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D115">
-        <v>393</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="B116" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="C116">
-        <v>1</v>
+        <v>1664</v>
       </c>
       <c r="D116">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>239</v>
+        <v>207</v>
       </c>
       <c r="B117" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
       <c r="C117">
-        <v>1264</v>
-      </c>
-      <c r="D117" t="s">
-        <v>401</v>
+        <v>96</v>
+      </c>
+      <c r="D117">
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="B118" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="C118">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D118">
-        <v>169</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B119" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C119">
-        <v>2</v>
-      </c>
-      <c r="D119" t="s">
-        <v>401</v>
+        <v>4</v>
+      </c>
+      <c r="D119">
+        <v>98</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="B120" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C120">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D120">
-        <v>250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B121" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C121">
-        <v>4</v>
-      </c>
-      <c r="D121" t="s">
-        <v>401</v>
+        <v>84</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B122" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C122">
-        <v>1</v>
-      </c>
-      <c r="D122" t="s">
-        <v>401</v>
+        <v>2</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B123" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C123">
-        <v>1</v>
-      </c>
-      <c r="D123" t="s">
-        <v>401</v>
+        <v>18</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B124" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C124">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="D124">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="B125" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="C125">
-        <v>4666</v>
-      </c>
-      <c r="D125" t="s">
-        <v>401</v>
+        <v>1</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="B126" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="C126">
-        <v>96</v>
-      </c>
-      <c r="D126" t="s">
-        <v>401</v>
+        <v>1</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B127" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="C127">
-        <v>18</v>
-      </c>
-      <c r="D127" t="s">
-        <v>401</v>
+        <v>1</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="B128" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="C128">
-        <v>42</v>
-      </c>
-      <c r="D128" t="s">
-        <v>401</v>
+        <v>30</v>
+      </c>
+      <c r="D128">
+        <v>64</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>205</v>
+        <v>231</v>
       </c>
       <c r="B129" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="C129">
-        <v>1664</v>
+        <v>139</v>
       </c>
       <c r="D129">
-        <v>634</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B130" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C130">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D130">
-        <v>249</v>
+        <v>42</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B131" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C131">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D131">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>384</v>
+        <v>237</v>
       </c>
       <c r="B132" t="s">
-        <v>414</v>
-      </c>
-      <c r="C132" t="s">
-        <v>401</v>
+        <v>238</v>
+      </c>
+      <c r="C132">
+        <v>4666</v>
       </c>
       <c r="D132">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="B133" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="C133">
-        <v>50</v>
-      </c>
-      <c r="D133" t="s">
-        <v>401</v>
+        <v>1264</v>
+      </c>
+      <c r="D133">
+        <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="B134" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="C134">
-        <v>654</v>
-      </c>
-      <c r="D134" t="s">
-        <v>401</v>
+        <v>20</v>
+      </c>
+      <c r="D134">
+        <v>62</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B135" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C135">
-        <v>2</v>
-      </c>
-      <c r="D135" t="s">
-        <v>401</v>
+        <v>13</v>
+      </c>
+      <c r="D135">
+        <v>17</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="B136" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="C136">
-        <v>125</v>
-      </c>
-      <c r="D136" t="s">
-        <v>401</v>
+        <v>2</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B137" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C137">
-        <v>7</v>
-      </c>
-      <c r="D137" t="s">
-        <v>401</v>
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <v>95</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>247</v>
+        <v>383</v>
       </c>
       <c r="B138" t="s">
-        <v>248</v>
-      </c>
-      <c r="C138">
-        <v>1</v>
+        <v>413</v>
+      </c>
+      <c r="C138" t="s">
+        <v>401</v>
       </c>
       <c r="D138">
-        <v>375</v>
+        <v>18</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -5962,358 +6021,358 @@
       <c r="C139">
         <v>814</v>
       </c>
-      <c r="D139" t="s">
-        <v>401</v>
+      <c r="D139">
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>385</v>
+        <v>251</v>
       </c>
       <c r="B140" t="s">
-        <v>415</v>
-      </c>
-      <c r="C140" t="s">
-        <v>401</v>
+        <v>252</v>
+      </c>
+      <c r="C140">
+        <v>7</v>
       </c>
       <c r="D140">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>383</v>
+        <v>253</v>
       </c>
       <c r="B141" t="s">
-        <v>413</v>
-      </c>
-      <c r="C141" t="s">
-        <v>401</v>
+        <v>254</v>
+      </c>
+      <c r="C141">
+        <v>654</v>
       </c>
       <c r="D141">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
       <c r="B142" t="s">
-        <v>224</v>
+        <v>256</v>
       </c>
       <c r="C142">
-        <v>1</v>
-      </c>
-      <c r="D142" t="s">
-        <v>401</v>
+        <v>417</v>
+      </c>
+      <c r="D142">
+        <v>4</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B143" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C143">
-        <v>417</v>
-      </c>
-      <c r="D143" t="s">
-        <v>401</v>
+        <v>50</v>
+      </c>
+      <c r="D143">
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>261</v>
+        <v>384</v>
       </c>
       <c r="B144" t="s">
-        <v>262</v>
-      </c>
-      <c r="C144">
-        <v>87</v>
-      </c>
-      <c r="D144" t="s">
+        <v>414</v>
+      </c>
+      <c r="C144" t="s">
         <v>401</v>
+      </c>
+      <c r="D144">
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>273</v>
+        <v>385</v>
       </c>
       <c r="B145" t="s">
-        <v>274</v>
-      </c>
-      <c r="C145">
-        <v>611</v>
-      </c>
-      <c r="D145" t="s">
+        <v>415</v>
+      </c>
+      <c r="C145" t="s">
         <v>401</v>
+      </c>
+      <c r="D145">
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="B146" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="C146">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="D146">
-        <v>73</v>
+        <v>7</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B147" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C147">
-        <v>208</v>
+        <v>87</v>
       </c>
       <c r="D147">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B148" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C148">
-        <v>2</v>
+        <v>208</v>
       </c>
       <c r="D148">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="B149" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="C149">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="D149">
-        <v>95</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B150" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C150">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="D150">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B151" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C151">
-        <v>256</v>
-      </c>
-      <c r="D151" t="s">
-        <v>401</v>
+        <v>2</v>
+      </c>
+      <c r="D151">
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B152" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C152">
-        <v>1562</v>
-      </c>
-      <c r="D152" t="s">
-        <v>401</v>
+        <v>256</v>
+      </c>
+      <c r="D152">
+        <v>7</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B153" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C153">
-        <v>340</v>
-      </c>
-      <c r="D153" t="s">
-        <v>401</v>
+        <v>611</v>
+      </c>
+      <c r="D153">
+        <v>7</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B154" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C154">
-        <v>75</v>
-      </c>
-      <c r="D154" t="s">
-        <v>401</v>
+        <v>1562</v>
+      </c>
+      <c r="D154">
+        <v>27</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>285</v>
+        <v>386</v>
       </c>
       <c r="B155" t="s">
-        <v>286</v>
-      </c>
-      <c r="C155">
-        <v>135</v>
-      </c>
-      <c r="D155" t="s">
+        <v>416</v>
+      </c>
+      <c r="C155" t="s">
         <v>401</v>
+      </c>
+      <c r="D155">
+        <v>6</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="B156" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="C156">
-        <v>4</v>
-      </c>
-      <c r="D156" t="s">
-        <v>401</v>
+        <v>75</v>
+      </c>
+      <c r="D156">
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="B157" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C157">
-        <v>1649</v>
-      </c>
-      <c r="D157" t="s">
-        <v>401</v>
+        <v>43</v>
+      </c>
+      <c r="D157">
+        <v>20</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B158" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="C158">
-        <v>29494</v>
-      </c>
-      <c r="D158" t="s">
-        <v>401</v>
+        <v>340</v>
+      </c>
+      <c r="D158">
+        <v>6</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>388</v>
+        <v>283</v>
       </c>
       <c r="B159" t="s">
-        <v>418</v>
-      </c>
-      <c r="C159" t="s">
-        <v>401</v>
+        <v>284</v>
+      </c>
+      <c r="C159">
+        <v>80</v>
       </c>
       <c r="D159">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>191</v>
+        <v>285</v>
       </c>
       <c r="B160" t="s">
-        <v>192</v>
+        <v>286</v>
       </c>
       <c r="C160">
-        <v>6</v>
+        <v>135</v>
       </c>
       <c r="D160">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>386</v>
+        <v>287</v>
       </c>
       <c r="B161" t="s">
-        <v>416</v>
-      </c>
-      <c r="C161" t="s">
-        <v>401</v>
+        <v>288</v>
+      </c>
+      <c r="C161">
+        <v>4</v>
       </c>
       <c r="D161">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>395</v>
+        <v>289</v>
       </c>
       <c r="B162" t="s">
-        <v>425</v>
-      </c>
-      <c r="C162" t="s">
-        <v>401</v>
+        <v>290</v>
+      </c>
+      <c r="C162">
+        <v>1649</v>
       </c>
       <c r="D162">
-        <v>148</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="B163" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="C163">
-        <v>4</v>
+        <v>267</v>
       </c>
       <c r="D163">
-        <v>58</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
       <c r="B164" t="s">
-        <v>320</v>
+        <v>294</v>
       </c>
       <c r="C164">
-        <v>1</v>
-      </c>
-      <c r="D164" t="s">
-        <v>401</v>
+        <v>29494</v>
+      </c>
+      <c r="D164">
+        <v>45</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -6327,63 +6386,63 @@
         <v>207</v>
       </c>
       <c r="D165">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>313</v>
+        <v>387</v>
       </c>
       <c r="B166" t="s">
-        <v>314</v>
-      </c>
-      <c r="C166">
-        <v>37</v>
-      </c>
-      <c r="D166" t="s">
+        <v>417</v>
+      </c>
+      <c r="C166" t="s">
         <v>401</v>
+      </c>
+      <c r="D166">
+        <v>104</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="B167" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="C167">
-        <v>267</v>
-      </c>
-      <c r="D167" t="s">
-        <v>401</v>
+        <v>3</v>
+      </c>
+      <c r="D167">
+        <v>60</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B168" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C168">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D168">
-        <v>239</v>
+        <v>40</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B169" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C169">
+        <v>2908</v>
+      </c>
+      <c r="D169">
         <v>2</v>
-      </c>
-      <c r="D169">
-        <v>29</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -6396,176 +6455,176 @@
       <c r="C170">
         <v>1358</v>
       </c>
-      <c r="D170" t="s">
-        <v>401</v>
+      <c r="D170">
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>323</v>
+        <v>388</v>
       </c>
       <c r="B171" t="s">
-        <v>324</v>
-      </c>
-      <c r="C171">
-        <v>2</v>
-      </c>
-      <c r="D171" t="s">
+        <v>418</v>
+      </c>
+      <c r="C171" t="s">
         <v>401</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B172" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C172">
-        <v>90</v>
-      </c>
-      <c r="D172" t="s">
-        <v>401</v>
+        <v>80</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B173" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C173">
-        <v>80</v>
-      </c>
-      <c r="D173" t="s">
-        <v>401</v>
+        <v>90</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>387</v>
+        <v>309</v>
       </c>
       <c r="B174" t="s">
-        <v>417</v>
-      </c>
-      <c r="C174" t="s">
-        <v>401</v>
+        <v>310</v>
+      </c>
+      <c r="C174">
+        <v>2</v>
       </c>
       <c r="D174">
-        <v>416</v>
+        <v>7</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B175" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C175">
-        <v>5</v>
-      </c>
-      <c r="D175" t="s">
-        <v>401</v>
+        <v>4</v>
+      </c>
+      <c r="D175">
+        <v>15</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>368</v>
+        <v>313</v>
       </c>
       <c r="B176" t="s">
-        <v>369</v>
+        <v>314</v>
       </c>
       <c r="C176">
-        <v>672</v>
+        <v>37</v>
       </c>
       <c r="D176">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>376</v>
+        <v>315</v>
       </c>
       <c r="B177" t="s">
-        <v>406</v>
-      </c>
-      <c r="C177" t="s">
-        <v>401</v>
+        <v>316</v>
+      </c>
+      <c r="C177">
+        <v>5</v>
       </c>
       <c r="D177">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>104</v>
+        <v>317</v>
       </c>
       <c r="B178" t="s">
-        <v>105</v>
+        <v>318</v>
       </c>
       <c r="C178">
-        <v>1454</v>
-      </c>
-      <c r="D178" t="s">
-        <v>401</v>
+        <v>31</v>
+      </c>
+      <c r="D178">
+        <v>45</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>193</v>
+        <v>319</v>
       </c>
       <c r="B179" t="s">
-        <v>194</v>
+        <v>320</v>
       </c>
       <c r="C179">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="D179">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>356</v>
+        <v>321</v>
       </c>
       <c r="B180" t="s">
-        <v>357</v>
+        <v>322</v>
       </c>
       <c r="C180">
-        <v>2</v>
-      </c>
-      <c r="D180" t="s">
-        <v>401</v>
+        <v>15</v>
+      </c>
+      <c r="D180">
+        <v>12</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="B181" t="s">
-        <v>300</v>
+        <v>324</v>
       </c>
       <c r="C181">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D181">
-        <v>161</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="B182" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="C182">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="D182">
-        <v>181</v>
+        <v>71</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -6579,329 +6638,329 @@
         <v>1</v>
       </c>
       <c r="D183">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>301</v>
+        <v>389</v>
       </c>
       <c r="B184" t="s">
-        <v>302</v>
-      </c>
-      <c r="C184">
-        <v>2908</v>
-      </c>
-      <c r="D184" t="s">
+        <v>419</v>
+      </c>
+      <c r="C184" t="s">
         <v>401</v>
+      </c>
+      <c r="D184">
+        <v>17</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>64</v>
+        <v>329</v>
       </c>
       <c r="B185" t="s">
-        <v>65</v>
+        <v>330</v>
       </c>
       <c r="C185">
-        <v>128</v>
-      </c>
-      <c r="D185" t="s">
-        <v>401</v>
+        <v>5</v>
+      </c>
+      <c r="D185">
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="B186" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="C186">
-        <v>6</v>
+        <v>1769</v>
       </c>
       <c r="D186">
-        <v>283</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="B187" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="C187">
-        <v>4270</v>
-      </c>
-      <c r="D187" t="s">
-        <v>401</v>
+        <v>12</v>
+      </c>
+      <c r="D187">
+        <v>47</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>333</v>
+        <v>390</v>
       </c>
       <c r="B188" t="s">
-        <v>334</v>
-      </c>
-      <c r="C188">
-        <v>12</v>
+        <v>420</v>
+      </c>
+      <c r="C188" t="s">
+        <v>401</v>
       </c>
       <c r="D188">
-        <v>183</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>345</v>
+        <v>391</v>
       </c>
       <c r="B189" t="s">
-        <v>346</v>
-      </c>
-      <c r="C189">
-        <v>18</v>
-      </c>
-      <c r="D189" t="s">
+        <v>421</v>
+      </c>
+      <c r="C189" t="s">
         <v>401</v>
+      </c>
+      <c r="D189">
+        <v>47</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B190" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C190">
-        <v>1769</v>
-      </c>
-      <c r="D190" t="s">
-        <v>401</v>
+        <v>420</v>
+      </c>
+      <c r="D190">
+        <v>113</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>390</v>
+        <v>337</v>
       </c>
       <c r="B191" t="s">
-        <v>420</v>
-      </c>
-      <c r="C191" t="s">
-        <v>401</v>
+        <v>338</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
       </c>
       <c r="D191">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="B192" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="C192">
-        <v>5</v>
-      </c>
-      <c r="D192" t="s">
-        <v>401</v>
+        <v>5089</v>
+      </c>
+      <c r="D192">
+        <v>13</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B193" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="C193">
-        <v>1</v>
-      </c>
-      <c r="D193" t="s">
-        <v>401</v>
+        <v>50</v>
+      </c>
+      <c r="D193">
+        <v>22</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B194" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C194">
-        <v>50</v>
+        <v>4270</v>
       </c>
       <c r="D194">
-        <v>83</v>
+        <v>5</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="B195" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="C195">
-        <v>420</v>
+        <v>18</v>
       </c>
       <c r="D195">
-        <v>451</v>
+        <v>3</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="B196" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="C196">
-        <v>5089</v>
+        <v>1329</v>
       </c>
       <c r="D196">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>391</v>
+        <v>349</v>
       </c>
       <c r="B197" t="s">
-        <v>421</v>
-      </c>
-      <c r="C197" t="s">
-        <v>401</v>
+        <v>350</v>
+      </c>
+      <c r="C197">
+        <v>9</v>
       </c>
       <c r="D197">
-        <v>189</v>
+        <v>5</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>349</v>
+        <v>392</v>
       </c>
       <c r="B198" t="s">
-        <v>350</v>
-      </c>
-      <c r="C198">
-        <v>9</v>
+        <v>422</v>
+      </c>
+      <c r="C198" t="s">
+        <v>401</v>
       </c>
       <c r="D198">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="B199" t="s">
-        <v>348</v>
+        <v>437</v>
       </c>
       <c r="C199">
-        <v>1329</v>
-      </c>
-      <c r="D199" t="s">
-        <v>401</v>
+        <v>9695</v>
+      </c>
+      <c r="D199">
+        <v>384</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>2</v>
+        <v>352</v>
       </c>
       <c r="B200" t="s">
-        <v>3</v>
+        <v>353</v>
       </c>
       <c r="C200">
-        <v>428</v>
-      </c>
-      <c r="D200" t="s">
-        <v>401</v>
+        <v>728</v>
+      </c>
+      <c r="D200">
+        <v>7</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>116</v>
+        <v>354</v>
       </c>
       <c r="B201" t="s">
-        <v>436</v>
+        <v>355</v>
       </c>
       <c r="C201">
-        <v>1481</v>
-      </c>
-      <c r="D201" t="s">
-        <v>401</v>
+        <v>20</v>
+      </c>
+      <c r="D201">
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>392</v>
+        <v>356</v>
       </c>
       <c r="B202" t="s">
-        <v>422</v>
-      </c>
-      <c r="C202" t="s">
-        <v>401</v>
+        <v>357</v>
+      </c>
+      <c r="C202">
+        <v>2</v>
       </c>
       <c r="D202">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="B203" t="s">
-        <v>437</v>
+        <v>359</v>
       </c>
       <c r="C203">
-        <v>9695</v>
-      </c>
-      <c r="D203" t="s">
-        <v>401</v>
+        <v>878</v>
+      </c>
+      <c r="D203">
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B204" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C204">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D204">
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="B205" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="C205">
-        <v>728</v>
+        <v>2</v>
       </c>
       <c r="D205">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="B206" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="C206">
-        <v>20</v>
-      </c>
-      <c r="D206" t="s">
-        <v>401</v>
+        <v>6315</v>
+      </c>
+      <c r="D206">
+        <v>3</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -6915,63 +6974,63 @@
         <v>401</v>
       </c>
       <c r="D207">
-        <v>97</v>
+        <v>24</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>358</v>
+        <v>394</v>
       </c>
       <c r="B208" t="s">
-        <v>359</v>
-      </c>
-      <c r="C208">
-        <v>878</v>
-      </c>
-      <c r="D208" t="s">
+        <v>424</v>
+      </c>
+      <c r="C208" t="s">
         <v>401</v>
+      </c>
+      <c r="D208">
+        <v>30</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>364</v>
+        <v>395</v>
       </c>
       <c r="B209" t="s">
-        <v>365</v>
-      </c>
-      <c r="C209">
-        <v>6315</v>
-      </c>
-      <c r="D209" t="s">
+        <v>425</v>
+      </c>
+      <c r="C209" t="s">
         <v>401</v>
+      </c>
+      <c r="D209">
+        <v>37</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>394</v>
+        <v>366</v>
       </c>
       <c r="B210" t="s">
-        <v>424</v>
-      </c>
-      <c r="C210" t="s">
-        <v>401</v>
+        <v>367</v>
+      </c>
+      <c r="C210">
+        <v>2</v>
       </c>
       <c r="D210">
-        <v>120</v>
+        <v>10</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B211" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C211">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="D211">
-        <v>41</v>
+        <v>17</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -6985,7 +7044,7 @@
         <v>21</v>
       </c>
       <c r="D212">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -6999,7 +7058,7 @@
         <v>401</v>
       </c>
       <c r="D213">
-        <v>87</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added formula for spearman's rank
</commit_message>
<xml_diff>
--- a/data/Malicious Routing Shortlist.xlsx
+++ b/data/Malicious Routing Shortlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikna\Desktop\Politics of Routing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086A317B-A3A6-47A6-90CA-838E3B1816DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2322FDE-2800-4A2A-B2CD-EA2AE66B1A5C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="446">
   <si>
     <t>AD</t>
   </si>
@@ -1363,13 +1363,7 @@
     <t>Number of independent routing paths</t>
   </si>
   <si>
-    <t>Proximity to hegemonic nations</t>
-  </si>
-  <si>
     <t>Mirai-Like attacker/victim</t>
-  </si>
-  <si>
-    <t>Exposure to nearby nations conducting mass surveillance.2</t>
   </si>
   <si>
     <t>Exposure to major surveillance scheme by proximity</t>
@@ -1917,9 +1911,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{442F76CE-3F66-42BB-AD05-A29D1E28F0FF}" name="Table3" displayName="Table3" ref="A1:K67" totalsRowCount="1">
-  <autoFilter ref="A1:K66" xr:uid="{5D7A7C19-206F-4AA4-8764-1A67075BA007}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{442F76CE-3F66-42BB-AD05-A29D1E28F0FF}" name="Table3" displayName="Table3" ref="A1:I67" totalsRowCount="1">
+  <autoFilter ref="A1:I66" xr:uid="{5D7A7C19-206F-4AA4-8764-1A67075BA007}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{6CAE0BB8-B52D-4A20-9ADF-6A97394DE9AD}" name="Country"/>
     <tableColumn id="11" xr3:uid="{E090A22D-FB18-4748-A91D-414C31BC34CD}" name="Exposure to major surveillance scheme by proximity"/>
     <tableColumn id="2" xr3:uid="{3CED1D76-1951-4C3A-814D-035739A9FCBB}" name="Mirai-Like attacker/victim" totalsRowFunction="custom">
@@ -1933,8 +1927,6 @@
     <tableColumn id="5" xr3:uid="{E8D3BBBC-FD07-4637-8DED-2FE5C7491C7E}" name="Citizens arrested over political social media posts"/>
     <tableColumn id="6" xr3:uid="{0A948547-E070-4D9E-A4DC-3394201B9DF2}" name="Any Internet/Telecom mass surveillance"/>
     <tableColumn id="3" xr3:uid="{117857E3-94F2-428B-901B-0A65A2DC9A2E}" name="Number of independent routing paths"/>
-    <tableColumn id="4" xr3:uid="{C77F7C6C-3FDB-46D9-AF53-A5FA9BCD762D}" name="Proximity to hegemonic nations"/>
-    <tableColumn id="8" xr3:uid="{A3BC02F8-FAD8-4507-9BC4-F7F494F9FACF}" name="Exposure to nearby nations conducting mass surveillance.2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2253,32 +2245,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA10CC7E-88B4-4460-87C0-163097071846}">
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18" customWidth="1"/>
     <col min="3" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
     <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>400</v>
       </c>
       <c r="B1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D1" t="s">
         <v>441</v>
@@ -2298,19 +2288,13 @@
       <c r="I1" t="s">
         <v>443</v>
       </c>
-      <c r="J1" t="s">
-        <v>444</v>
-      </c>
-      <c r="K1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>9</v>
@@ -2332,7 +2316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2359,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2386,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2413,7 +2397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>427</v>
       </c>
@@ -2440,12 +2424,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>41</v>
@@ -2467,7 +2451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2494,7 +2478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -2521,7 +2505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -2548,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>178</v>
       </c>
@@ -2575,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -2602,7 +2586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -2629,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -2656,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>428</v>
       </c>
@@ -2683,7 +2667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>99</v>
       </c>
@@ -2823,7 +2807,7 @@
         <v>128</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>6</v>
@@ -4091,7 +4075,7 @@
   <dimension ref="A1:D213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>